<commit_message>
Add new properties for customer order details
Updated OrderDetailModel to include CustomerSaleOrder, CustomerLocation, ItemModel, and CustItemCategory.
Modified SaleOrderDAL to retrieve and populate these new fields.
Enhanced SaleOrderController to process the new properties and added corresponding columns in the data table.
Updated OrderDetail.cshtml to include input fields and table headers for the new properties.
Adjusted JavaScript to send new data via AJAX and updated _SaleItemGrid.cshtml to display the additional information.
</commit_message>
<xml_diff>
--- a/eTactWeb/wwwroot/Uploads/ImportSaleOrderFormat.xlsx
+++ b/eTactWeb/wwwroot/Uploads/ImportSaleOrderFormat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soumitra\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erp\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00391C4-0CB7-4278-ADEF-4C74EE058946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778F7E20-31BE-4E27-A2D9-FA2356739B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Part Code</t>
   </si>
@@ -43,10 +43,13 @@
     <t>Date</t>
   </si>
   <si>
-    <t>FGAL0001</t>
-  </si>
-  <si>
-    <t>AAA</t>
+    <t>0001-908</t>
+  </si>
+  <si>
+    <t>aqa</t>
+  </si>
+  <si>
+    <t>dsf</t>
   </si>
 </sst>
 </file>
@@ -82,8 +85,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,12 +430,15 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -454,7 +461,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -462,10 +469,19 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>12</v>
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>45292</v>
       </c>
     </row>
   </sheetData>

</xml_diff>